<commit_message>
Modulo 1: Leccion1 VBA-Agregando Teoria
</commit_message>
<xml_diff>
--- a/Macros/DesarrolladorPractice1.xlsx
+++ b/Macros/DesarrolladorPractice1.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuch\OneDrive\Escritorio\EXCEL\Macros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95FBD293-64B7-49E4-9675-6D25C04921F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F6ADC3-54BC-4F28-B476-3787DD2C174B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{963E7C5F-44B2-46CF-AE45-FC0F1BBD83B7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Developer" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>🔹 How to Enable the Developer Tab in Excel (English version)</t>
   </si>
@@ -350,13 +350,188 @@
       </rPr>
       <t>.</t>
     </r>
+  </si>
+  <si>
+    <t>📖 Lección 1: ¿Qué es VBA y cómo funciona en Excel?</t>
+  </si>
+  <si>
+    <t>1️⃣ ¿Qué es VBA?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">VBA (Visual Basic for Applications) es un lenguaje de programación que permite </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>automatizar tareas repetitivas en Excel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> y otros programas de Microsoft Office (Word, PowerPoint, Outlook, etc.). Con VBA, podemos </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>crear macros</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, que son secuencias de instrucciones que Excel ejecuta automáticamente.</t>
+    </r>
+  </si>
+  <si>
+    <t>Ventajas de VBA</t>
+  </si>
+  <si>
+    <t>✅ Automatización de tareas repetitivas (formateo, cálculos, reportes).</t>
+  </si>
+  <si>
+    <t>✅ Reducción de errores manuales.</t>
+  </si>
+  <si>
+    <t>✅ Integración con bases de datos, Outlook y otros sistemas.</t>
+  </si>
+  <si>
+    <t>✅ Creación de funciones personalizadas que no existen en Excel.</t>
+  </si>
+  <si>
+    <r>
+      <t>Ejemplo:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Si todos los días copias datos de una hoja a otra, les das formato y los ordenas, VBA puede hacer todo eso con un solo clic.</t>
+    </r>
+  </si>
+  <si>
+    <t>2️⃣ Diferencias entre Macros Grabadas y Macros Programadas</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Antes de escribir código, Excel nos permite </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>grabar una macro</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sin necesidad de programar.</t>
+    </r>
+  </si>
+  <si>
+    <t>Tipo de Macro</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>Cuándo usarla</t>
+  </si>
+  <si>
+    <t>Grabada</t>
+  </si>
+  <si>
+    <t>Se registra paso a paso lo que hacemos en Excel.</t>
+  </si>
+  <si>
+    <t>Para tareas simples y repetitivas (ej. aplicar formato a celdas).</t>
+  </si>
+  <si>
+    <t>Programada (VBA)</t>
+  </si>
+  <si>
+    <t>Se escribe código para realizar tareas más complejas y dinámicas.</t>
+  </si>
+  <si>
+    <t>Cuando necesitamos condiciones, cálculos avanzados o automatización inteligente.</t>
+  </si>
+  <si>
+    <t>Ejemplo:</t>
+  </si>
+  <si>
+    <r>
+      <t>Macro grabada:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Guardar un formato de tabla y aplicarlo con un botón.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Macro programada:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Validar datos, hacer cálculos y generar reportes automáticamente.</t>
+    </r>
+  </si>
+  <si>
+    <t>SS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -388,6 +563,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -409,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -419,6 +602,27 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -754,10 +958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E567E402-4FD8-424B-808B-054797F4466A}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,6 +1032,121 @@
         <v>13</v>
       </c>
     </row>
+    <row r="15" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="9"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>